<commit_message>
Adds typeface.js for timing conversion
</commit_message>
<xml_diff>
--- a/Media/Statistics.xlsx
+++ b/Media/Statistics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="0" windowWidth="25860" windowHeight="23480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="25860" windowHeight="23480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -496,6 +496,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -515,11 +523,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -558,19 +561,32 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="21">
     <cellStyle name="Accent5" xfId="8" builtinId="45"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -912,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -923,25 +939,25 @@
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
@@ -960,92 +976,116 @@
       <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="2">
+        <v>79</v>
+      </c>
+      <c r="K2" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D3" s="2">
-        <v>233</v>
+        <v>1449</v>
       </c>
       <c r="E3" s="4">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4">
-        <v>190</v>
+        <v>935</v>
       </c>
       <c r="G3" s="6">
         <f>(C3-E3)/C3</f>
-        <v>0.2</v>
+        <v>0.41772151898734178</v>
       </c>
       <c r="H3" s="6">
         <f>(D3-F3)/D3</f>
-        <v>0.18454935622317598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.35472739820565907</v>
+      </c>
+      <c r="J3" s="2">
+        <v>39</v>
+      </c>
+      <c r="K3" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2">
-        <v>310</v>
+        <v>611</v>
       </c>
       <c r="E4" s="4">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4">
-        <v>243</v>
+        <v>409</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G20" si="0">(C4-E4)/C4</f>
-        <v>0.21052631578947367</v>
+        <f>(C4-E4)/C4</f>
+        <v>0.41025641025641024</v>
       </c>
       <c r="H4" s="6">
-        <f t="shared" ref="H4:H20" si="1">(D4-F4)/D4</f>
-        <v>0.21612903225806451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <f>(D4-F4)/D4</f>
+        <v>0.33060556464811786</v>
+      </c>
+      <c r="J4" s="2">
+        <v>54</v>
+      </c>
+      <c r="K4" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2">
-        <v>286</v>
+        <v>1233</v>
       </c>
       <c r="E5" s="4">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F5" s="4">
-        <v>248</v>
+        <v>755</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>0.21428571428571427</v>
+        <f>(C5-E5)/C5</f>
+        <v>0.40740740740740738</v>
       </c>
       <c r="H5" s="6">
-        <f t="shared" si="1"/>
-        <v>0.13286713286713286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <f>(D5-F5)/D5</f>
+        <v>0.38767234387672345</v>
+      </c>
+      <c r="J5" s="2">
+        <v>29</v>
+      </c>
+      <c r="K5" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1065,71 +1105,77 @@
         <v>390</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="0"/>
+        <f>(C6-E6)/C6</f>
         <v>0.37931034482758619</v>
       </c>
       <c r="H6" s="6">
-        <f t="shared" si="1"/>
+        <f>(D6-F6)/D6</f>
         <v>0.38775510204081631</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6" s="2">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2">
+        <v>474</v>
+      </c>
+      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4">
+        <v>326</v>
+      </c>
+      <c r="G7" s="6">
+        <f>(C7-E7)/C7</f>
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="H7" s="6">
+        <f>(D7-F7)/D7</f>
+        <v>0.31223628691983124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>28</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>468</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>18</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F8" s="4">
         <v>299</v>
       </c>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
+      <c r="G8" s="6">
+        <f>(C8-E8)/C8</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="H7" s="6">
-        <f t="shared" si="1"/>
+      <c r="H8" s="6">
+        <f>(D8-F8)/D8</f>
         <v>0.3611111111111111</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2">
-        <v>400</v>
-      </c>
-      <c r="E8" s="4">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
-        <v>325</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="1"/>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1149,15 +1195,15 @@
         <v>333</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
+        <f>(C9-E9)/C9</f>
         <v>0.34482758620689657</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="1"/>
+        <f>(D9-F9)/D9</f>
         <v>0.32317073170731708</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1177,127 +1223,127 @@
         <v>451</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
+        <f>(C10-E10)/C10</f>
         <v>0.34285714285714286</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" si="1"/>
+        <f>(D10-F10)/D10</f>
         <v>0.31145038167938932</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:11">
       <c r="A11">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2">
-        <v>611</v>
+        <v>1850</v>
       </c>
       <c r="E11" s="4">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F11" s="4">
-        <v>409</v>
+        <v>1280</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.41025641025641024</v>
+        <f>(C11-E11)/C11</f>
+        <v>0.32307692307692309</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33060556464811786</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <f>(D11-F11)/D11</f>
+        <v>0.30810810810810813</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2">
+        <v>485</v>
+      </c>
+      <c r="E12" s="4">
+        <v>17</v>
+      </c>
+      <c r="F12" s="4">
+        <v>376</v>
+      </c>
+      <c r="G12" s="6">
+        <f>(C12-E12)/C12</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="H12" s="6">
+        <f>(D12-F12)/D12</f>
+        <v>0.22474226804123712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
+        <v>286</v>
+      </c>
+      <c r="E13" s="4">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4">
+        <v>248</v>
+      </c>
+      <c r="G13" s="6">
+        <f>(C13-E13)/C13</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="H13" s="6">
+        <f>(D13-F13)/D13</f>
+        <v>0.13286713286713286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
         <v>19</v>
       </c>
-      <c r="D12" s="2">
-        <v>474</v>
-      </c>
-      <c r="E12" s="4">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4">
-        <v>326</v>
-      </c>
-      <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>0.36842105263157893</v>
-      </c>
-      <c r="H12" s="6">
-        <f t="shared" si="1"/>
-        <v>0.31223628691983124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2">
-        <v>54</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1233</v>
-      </c>
-      <c r="E13" s="4">
-        <v>32</v>
-      </c>
-      <c r="F13" s="4">
-        <v>755</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>0.40740740740740738</v>
-      </c>
-      <c r="H13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.38767234387672345</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <v>79</v>
-      </c>
       <c r="D14" s="2">
-        <v>1449</v>
+        <v>310</v>
       </c>
       <c r="E14" s="4">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F14" s="4">
-        <v>935</v>
+        <v>243</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>0.41772151898734178</v>
+        <f>(C14-E14)/C14</f>
+        <v>0.21052631578947367</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="1"/>
-        <v>0.35472739820565907</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1">
+        <f>(D14-F14)/D14</f>
+        <v>0.21612903225806451</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1306,15 +1352,15 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="6" t="e">
-        <f t="shared" si="0"/>
+        <f>(C15-E15)/C15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H15" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f>(D15-F15)/D15</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1323,40 +1369,40 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="6" t="e">
-        <f t="shared" si="0"/>
+        <f>(C16-E16)/C16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H16" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f>(D16-F16)/D16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
-        <v>1850</v>
+        <v>233</v>
       </c>
       <c r="E17" s="4">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F17" s="4">
-        <v>1280</v>
+        <v>190</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="0"/>
-        <v>0.32307692307692309</v>
+        <f>(C17-E17)/C17</f>
+        <v>0.2</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="1"/>
-        <v>0.30810810810810813</v>
+        <f>(D17-F17)/D17</f>
+        <v>0.18454935622317598</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1379,11 +1425,11 @@
         <v>802</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="0"/>
+        <f>(C18-E18)/C18</f>
         <v>0.1951219512195122</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="1"/>
+        <f>(D18-F18)/D18</f>
         <v>0.19315895372233399</v>
       </c>
     </row>
@@ -1407,40 +1453,40 @@
         <v>184</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="0"/>
+        <f>(C19-E19)/C19</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="1"/>
+        <f>(D19-F19)/D19</f>
         <v>0.31598513011152418</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2">
-        <v>22</v>
-      </c>
       <c r="D20" s="2">
-        <v>485</v>
+        <v>400</v>
       </c>
       <c r="E20" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4">
-        <v>376</v>
+        <v>325</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="0"/>
-        <v>0.22727272727272727</v>
+        <f>(C20-E20)/C20</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="1"/>
-        <v>0.22474226804123712</v>
+        <f>(D20-F20)/D20</f>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1">
@@ -1452,11 +1498,11 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="6" t="e">
-        <f t="shared" ref="G21:G23" si="2">(C21-E21)/C21</f>
+        <f t="shared" ref="G21:G23" si="0">(C21-E21)/C21</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H21" s="6" t="e">
-        <f t="shared" ref="H21:H23" si="3">(D21-F21)/D21</f>
+        <f t="shared" ref="H21:H23" si="1">(D21-F21)/D21</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1469,11 +1515,11 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1495,11 +1541,11 @@
         <v>7546</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.32684824902723736</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.30425963488843816</v>
       </c>
     </row>
@@ -1509,38 +1555,144 @@
       </c>
       <c r="C24" s="10">
         <f>SUM(C6:C14)</f>
-        <v>330</v>
+        <v>260</v>
       </c>
       <c r="D24" s="10">
         <f>SUM(D6:D14)</f>
-        <v>6419</v>
+        <v>5657</v>
       </c>
       <c r="E24" s="11">
         <f>SUM(E6:E14)</f>
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="F24" s="11">
         <f>SUM(F6:F14)</f>
-        <v>4223</v>
+        <v>3946</v>
       </c>
       <c r="G24" s="12">
-        <f t="shared" ref="G24" si="4">(C24-E24)/C24</f>
-        <v>0.37272727272727274</v>
+        <f t="shared" ref="G24" si="2">(C24-E24)/C24</f>
+        <v>0.31923076923076921</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" ref="H24" si="5">(D24-F24)/D24</f>
-        <v>0.34210936282910109</v>
+        <f t="shared" ref="H24" si="3">(D24-F24)/D24</f>
+        <v>0.30245713275587766</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="E29">
+        <v>514</v>
+      </c>
+      <c r="F29">
+        <v>346</v>
+      </c>
+      <c r="G29">
+        <f>SUM(E29:F29)</f>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="E30">
+        <f>E29/G29</f>
+        <v>0.5976744186046512</v>
+      </c>
+      <c r="F30">
+        <f>F29/G29</f>
+        <v>0.40232558139534885</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7">
+      <c r="E34">
+        <v>260</v>
+      </c>
+      <c r="F34">
+        <v>177</v>
+      </c>
+      <c r="G34">
+        <f>SUM(E34:F34)</f>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7">
+      <c r="E35">
+        <f>E34/G34</f>
+        <v>0.59496567505720821</v>
+      </c>
+      <c r="F35">
+        <f>F34/G34</f>
+        <v>0.40503432494279173</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:H20">
+    <sortCondition descending="1" ref="G3:G20"/>
+    <sortCondition descending="1" ref="H3:H20"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C20">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6B226EF3-927A-264A-95DD-18B329682F04}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J6">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CC84EC44-0374-0E4C-89CB-959358C38DBE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6B226EF3-927A-264A-95DD-18B329682F04}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C3:C20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CC84EC44-0374-0E4C-89CB-959358C38DBE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J2:J6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -1564,132 +1716,132 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16" thickBot="1"/>
     <row r="2" spans="2:4" ht="18">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="2:4" ht="16" thickBot="1">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1709,7 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1721,91 +1873,91 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16" thickBot="1"/>
     <row r="2" spans="2:4" ht="18">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="33">
         <v>44</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="34">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="25">
         <v>7945</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="26">
         <v>1281</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="25">
         <v>943</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="26">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="27">
         <f>17*25+17+19</f>
         <v>461</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="28">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="25">
         <v>121</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="26">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16" thickBot="1">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="31" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>